<commit_message>
use-case-4: - added price asking info - corrected a malfunction of the form asking_required_info_to_user_form
</commit_message>
<xml_diff>
--- a/knowledge base/Chatbot_training_data.xlsx
+++ b/knowledge base/Chatbot_training_data.xlsx
@@ -1330,7 +1330,7 @@
   <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -9873,6 +9873,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050C83F05BD85FA4D93586BC3F742211B" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fde699bc0f2b799bf43d6bd792f8e6ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f09b5a9e-18c2-4c69-9941-8e5cec8a0026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3385c599266df4663eef3ee0cb43eba7" ns2:_="">
     <xsd:import namespace="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
@@ -10004,12 +10010,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10020,6 +10020,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB977730-9E92-4B6A-8F73-B1779EE87EA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0346AF-401D-4DD9-A208-2A4066E36256}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10037,22 +10053,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB977730-9E92-4B6A-8F73-B1779EE87EA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9200039-8C42-4E3A-8277-EB2F8E4B90D4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
use-case-5: - Not exactely what was asked but the idea is there
</commit_message>
<xml_diff>
--- a/knowledge base/Chatbot_training_data.xlsx
+++ b/knowledge base/Chatbot_training_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talan0-my.sharepoint.com/personal/lao-dja_tchala_talan_com/Documents/Formation Liebherr/Chatbot-Rasa/knowledge base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB31F66-3CB9-49A5-925A-C855AAC2F6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{5BB31F66-3CB9-49A5-925A-C855AAC2F6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{248DC572-B17A-4089-A7D5-317369CC55E4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1330,7 +1330,7 @@
   <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -9873,12 +9873,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050C83F05BD85FA4D93586BC3F742211B" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fde699bc0f2b799bf43d6bd792f8e6ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f09b5a9e-18c2-4c69-9941-8e5cec8a0026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3385c599266df4663eef3ee0cb43eba7" ns2:_="">
     <xsd:import namespace="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
@@ -10010,6 +10004,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10020,22 +10020,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB977730-9E92-4B6A-8F73-B1779EE87EA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0346AF-401D-4DD9-A208-2A4066E36256}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10053,6 +10037,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB977730-9E92-4B6A-8F73-B1779EE87EA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f09b5a9e-18c2-4c69-9941-8e5cec8a0026"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9200039-8C42-4E3A-8277-EB2F8E4B90D4}">
   <ds:schemaRefs>

</xml_diff>